<commit_message>
fixed hrgreen id,add coffee green logos
</commit_message>
<xml_diff>
--- a/www/data/iday14-full.xlsx
+++ b/www/data/iday14-full.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="1820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="grid" sheetId="1" r:id="rId1"/>
@@ -2716,9 +2716,6 @@
     <t>harley-davidson</t>
   </si>
   <si>
-    <t>hr-green</t>
-  </si>
-  <si>
     <t>hydra-force</t>
   </si>
   <si>
@@ -3005,6 +3002,9 @@
   </si>
   <si>
     <t>belvedere-trading</t>
+  </si>
+  <si>
+    <t>hrgreen</t>
   </si>
 </sst>
 </file>
@@ -3996,10 +3996,10 @@
   <dimension ref="A1:AC69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4028,7 +4028,7 @@
         <v>82</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>47</v>
@@ -4046,7 +4046,7 @@
         <v>85</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>88</v>
@@ -4055,43 +4055,43 @@
         <v>89</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>90</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>91</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>919</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>920</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>915</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>921</v>
-      </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>916</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>917</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>918</v>
       </c>
-      <c r="V1" s="5" t="s">
-        <v>919</v>
-      </c>
       <c r="W1" s="4" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="AA1" s="4" t="s">
         <v>276</v>
@@ -4100,7 +4100,7 @@
         <v>277</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="2" spans="1:29">
@@ -4309,7 +4309,7 @@
         <v>1240</v>
       </c>
       <c r="AC4" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="5" spans="1:29">
@@ -4375,7 +4375,7 @@
         <v>373</v>
       </c>
       <c r="AC5" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="6" spans="1:29">
@@ -4438,7 +4438,7 @@
         <v>396</v>
       </c>
       <c r="AC6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="7" spans="1:29">
@@ -4501,7 +4501,7 @@
         <v>1530</v>
       </c>
       <c r="AC7" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="8" spans="1:29">
@@ -4509,7 +4509,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -4564,7 +4564,7 @@
         <v>1586</v>
       </c>
       <c r="AC8" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="9" spans="1:29">
@@ -4702,7 +4702,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -4822,7 +4822,7 @@
         <v>960</v>
       </c>
       <c r="AC12" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="13" spans="1:29">
@@ -4885,7 +4885,7 @@
         <v>160</v>
       </c>
       <c r="AC13" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="14" spans="1:29">
@@ -4948,7 +4948,7 @@
         <v>1160</v>
       </c>
       <c r="AC14" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="15" spans="1:29">
@@ -5013,7 +5013,7 @@
         <v>904</v>
       </c>
       <c r="AC15" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="16" spans="1:29">
@@ -5141,7 +5141,7 @@
         <v>1026</v>
       </c>
       <c r="AC17" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="18" spans="1:29">
@@ -5149,7 +5149,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -5208,7 +5208,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -5268,7 +5268,7 @@
         <v>1508</v>
       </c>
       <c r="AC19" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="20" spans="1:29">
@@ -5331,7 +5331,7 @@
         <v>1227</v>
       </c>
       <c r="AC20" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="21" spans="1:29">
@@ -5396,7 +5396,7 @@
         <v>852</v>
       </c>
       <c r="AC21" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="22" spans="1:29">
@@ -5467,7 +5467,7 @@
         <v>118</v>
       </c>
       <c r="AC22" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="23" spans="1:29">
@@ -5475,7 +5475,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
@@ -5601,7 +5601,7 @@
         <v>1074</v>
       </c>
       <c r="AC24" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="25" spans="1:29">
@@ -5726,7 +5726,7 @@
         <v>336</v>
       </c>
       <c r="AC26" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="27" spans="1:29">
@@ -5789,7 +5789,7 @@
         <v>6</v>
       </c>
       <c r="AC27" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="28" spans="1:29">
@@ -5854,7 +5854,7 @@
         <v>922</v>
       </c>
       <c r="AC28" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="29" spans="1:29">
@@ -6045,7 +6045,7 @@
         <v>800</v>
       </c>
       <c r="AC31" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="32" spans="1:29">
@@ -6108,7 +6108,7 @@
         <v>1729</v>
       </c>
       <c r="AC32" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="33" spans="1:29">
@@ -6179,7 +6179,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>896</v>
+        <v>992</v>
       </c>
       <c r="C34" t="s">
         <v>32</v>
@@ -6242,7 +6242,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C35" t="s">
         <v>33</v>
@@ -6490,7 +6490,7 @@
         <v>717</v>
       </c>
       <c r="AC38" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="39" spans="1:29">
@@ -6498,7 +6498,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C39" t="s">
         <v>37</v>
@@ -6556,7 +6556,7 @@
         <v>1229</v>
       </c>
       <c r="AC39" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="40" spans="1:29">
@@ -6564,10 +6564,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C40" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D40" s="21">
         <v>0</v>
@@ -6621,7 +6621,7 @@
         <v>1628</v>
       </c>
       <c r="AC40" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="41" spans="1:29">
@@ -6684,7 +6684,7 @@
         <v>1274</v>
       </c>
       <c r="AC41" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="42" spans="1:29">
@@ -6692,7 +6692,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C42" t="s">
         <v>54</v>
@@ -6814,7 +6814,7 @@
         <v>999</v>
       </c>
       <c r="AC43" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="44" spans="1:29">
@@ -6879,7 +6879,7 @@
         <v>475</v>
       </c>
       <c r="AC44" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="45" spans="1:29">
@@ -6944,7 +6944,7 @@
         <v>46</v>
       </c>
       <c r="AC45" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="46" spans="1:29">
@@ -6952,7 +6952,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C46" t="s">
         <v>42</v>
@@ -7007,7 +7007,7 @@
         <v>17</v>
       </c>
       <c r="AC46" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="47" spans="1:29">
@@ -7139,7 +7139,7 @@
         <v>78</v>
       </c>
       <c r="AC48" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="49" spans="1:29">
@@ -7202,7 +7202,7 @@
         <v>1575</v>
       </c>
       <c r="AC49" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="50" spans="1:29">
@@ -7210,7 +7210,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C50" t="s">
         <v>46</v>
@@ -7275,10 +7275,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C51" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D51" s="12">
         <v>0</v>
@@ -7332,12 +7332,12 @@
         <v>117</v>
       </c>
       <c r="AC51" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="54" spans="1:29">
       <c r="C54" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -7361,7 +7361,7 @@
         <v>47</v>
       </c>
       <c r="B57" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="58" spans="1:29">
@@ -7369,7 +7369,7 @@
         <v>83</v>
       </c>
       <c r="B58" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="59" spans="1:29">
@@ -7377,7 +7377,7 @@
         <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="60" spans="1:29">
@@ -7385,7 +7385,7 @@
         <v>86</v>
       </c>
       <c r="B60" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="61" spans="1:29">
@@ -7393,15 +7393,15 @@
         <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="62" spans="1:29">
       <c r="A62" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B62" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="63" spans="1:29">
@@ -7409,7 +7409,7 @@
         <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="64" spans="1:29">
@@ -7417,15 +7417,15 @@
         <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B65" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -7433,15 +7433,15 @@
         <v>90</v>
       </c>
       <c r="B66" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B67" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -7449,15 +7449,15 @@
         <v>91</v>
       </c>
       <c r="B68" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B69" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
   </sheetData>
@@ -8675,7 +8675,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E9" s="9">
         <v>80</v>
@@ -8981,7 +8981,7 @@
         <v>904</v>
       </c>
       <c r="D15" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E15" s="9">
         <v>1461</v>
@@ -9723,7 +9723,7 @@
         <v>336</v>
       </c>
       <c r="D29" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E29" s="9">
         <v>797</v>
@@ -10264,7 +10264,7 @@
         <v>311</v>
       </c>
       <c r="D40" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="E40" s="9">
         <v>767</v>
@@ -11347,7 +11347,7 @@
         <v>117</v>
       </c>
       <c r="D61" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E61" s="9">
         <v>237</v>
@@ -12060,7 +12060,7 @@
         <v>753</v>
       </c>
       <c r="D74" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E74" s="9">
         <v>1300</v>
@@ -12225,7 +12225,7 @@
         <v>47</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>83</v>
@@ -12237,7 +12237,7 @@
         <v>86</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>87</v>
@@ -12249,58 +12249,58 @@
         <v>89</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="K1" s="19" t="s">
         <v>90</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="M1" s="19" t="s">
         <v>91</v>
       </c>
       <c r="N1" s="19" t="s">
+        <v>928</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>932</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>988</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>933</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>930</v>
+      </c>
+      <c r="U1" s="19" t="s">
+        <v>931</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>923</v>
+      </c>
+      <c r="X1" s="19" t="s">
+        <v>924</v>
+      </c>
+      <c r="Y1" s="19" t="s">
+        <v>925</v>
+      </c>
+      <c r="Z1" s="19" t="s">
+        <v>926</v>
+      </c>
+      <c r="AA1" s="19" t="s">
+        <v>927</v>
+      </c>
+      <c r="AB1" s="19" t="s">
         <v>929</v>
       </c>
-      <c r="P1" s="19" t="s">
-        <v>933</v>
-      </c>
-      <c r="Q1" s="19" t="s">
-        <v>989</v>
-      </c>
-      <c r="R1" s="19" t="s">
+      <c r="AD1" s="19" t="s">
+        <v>935</v>
+      </c>
+      <c r="AE1" s="19" t="s">
         <v>934</v>
-      </c>
-      <c r="T1" s="19" t="s">
-        <v>931</v>
-      </c>
-      <c r="U1" s="19" t="s">
-        <v>932</v>
-      </c>
-      <c r="W1" s="19" t="s">
-        <v>924</v>
-      </c>
-      <c r="X1" s="19" t="s">
-        <v>925</v>
-      </c>
-      <c r="Y1" s="19" t="s">
-        <v>926</v>
-      </c>
-      <c r="Z1" s="19" t="s">
-        <v>927</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>928</v>
-      </c>
-      <c r="AB1" s="19" t="s">
-        <v>930</v>
-      </c>
-      <c r="AD1" s="19" t="s">
-        <v>936</v>
-      </c>
-      <c r="AE1" s="19" t="s">
-        <v>935</v>
       </c>
     </row>
     <row r="2" spans="1:31">
@@ -15459,7 +15459,7 @@
     </row>
     <row r="40" spans="1:31">
       <c r="A40" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B40" s="21">
         <v>1</v>
@@ -16372,7 +16372,7 @@
     </row>
     <row r="51" spans="1:31">
       <c r="A51" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B51" s="12">
         <v>0</v>
@@ -16777,22 +16777,22 @@
         <v>89</v>
       </c>
       <c r="K3" s="37" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="L3" s="37" t="s">
         <v>90</v>
       </c>
       <c r="M3" s="37" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="N3" s="37" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="O3" s="37" t="s">
         <v>91</v>
       </c>
       <c r="P3" s="37" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="R3" s="19"/>
       <c r="S3" s="19"/>
@@ -29536,7 +29536,7 @@
         <v>347</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -29695,7 +29695,7 @@
         <v>163</v>
       </c>
       <c r="B30" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="31" spans="1:2">

</xml_diff>